<commit_message>
changed install instructions for building blocks
</commit_message>
<xml_diff>
--- a/scripts/pathway_testing/test_pathways.xlsx
+++ b/scripts/pathway_testing/test_pathways.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Will/Dropbox (Personal)/Python_Projects/retrobiocat_web/scripts/pathway_testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Will/Dropbox (Personal)/Python_Projects/retrobiocat/scripts/pathway_testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F79CC4-CB03-4C4F-B89B-A88C6131E889}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905844A0-C407-C446-8ACF-385994052220}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1016,7 +1016,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Website quality improvements 2
</commit_message>
<xml_diff>
--- a/scripts/pathway_testing/test_pathways.xlsx
+++ b/scripts/pathway_testing/test_pathways.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Will/Dropbox (Personal)/Python_Projects/retrobiocat/scripts/pathway_testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B471CC-D1DA-114D-9B27-E002C6648CB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0048FE6-3EB1-5B41-B02D-229DF032FB41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -961,11 +961,12 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="4" max="4" width="22.1640625" customWidth="1"/>
     <col min="5" max="5" width="35.6640625" customWidth="1"/>
     <col min="7" max="7" width="37.6640625" customWidth="1"/>
     <col min="8" max="8" width="27.1640625" customWidth="1"/>
@@ -1680,15 +1681,6 @@
       <c r="E28" t="s">
         <v>106</v>
       </c>
-      <c r="F28">
-        <v>3</v>
-      </c>
-      <c r="G28">
-        <v>3</v>
-      </c>
-      <c r="H28">
-        <v>3</v>
-      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">

</xml_diff>